<commit_message>
Popraw odliczanie kwoty wolnej po przekroczeniu progu
</commit_message>
<xml_diff>
--- a/polski-lad-netto.xlsx
+++ b/polski-lad-netto.xlsx
@@ -317,32 +317,7 @@
     <t xml:space="preserve">43,76 lub 0,00 jeśli brak PIT-2</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Sty: </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">85.528</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">zł lub 171.056zł wspólnie, zmiejsza się o PodstOp17</t>
-    </r>
+    <t xml:space="preserve">Sty: 85.528zł lub 171.056zł wspólnie, zmiejsza się o PodstOp17</t>
   </si>
   <si>
     <t xml:space="preserve">PodstOp*ProcPod/100%-UlgZmZal-SklZdrDoOdl</t>
@@ -357,7 +332,7 @@
     <numFmt numFmtId="165" formatCode="#,##0.00"/>
     <numFmt numFmtId="166" formatCode="0.00%"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -385,11 +360,6 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -507,10 +477,10 @@
       <selection pane="topRight" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="32.23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="32.22"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="52.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="3.08"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="9" min="5" style="1" width="11.52"/>
@@ -1845,52 +1815,52 @@
         <v>15</v>
       </c>
       <c r="E24" s="1" t="n">
-        <f aca="false">ROUND(MAX(E22*17%-E18,0)+E23*32%,0)</f>
+        <f aca="false">ROUND(MAX(E22*17%+E23*32%-E18,0),0)</f>
         <v>0</v>
       </c>
       <c r="F24" s="1" t="n">
-        <f aca="false">ROUND(MAX(F22*17%-F18,0)+F23*32%,0)</f>
+        <f aca="false">ROUND(MAX(F22*17%+F23*32%-F18,0),0)</f>
         <v>130</v>
       </c>
       <c r="G24" s="1" t="n">
-        <f aca="false">ROUND(MAX(G22*17%-G18,0)+G23*32%,0)</f>
+        <f aca="false">ROUND(MAX(G22*17%+G23*32%-G18,0),0)</f>
         <v>279</v>
       </c>
       <c r="H24" s="1" t="n">
-        <f aca="false">ROUND(MAX(H22*17%-H18,0)+H23*32%,0)</f>
+        <f aca="false">ROUND(MAX(H22*17%+H23*32%-H18,0),0)</f>
         <v>573</v>
       </c>
       <c r="I24" s="1" t="n">
-        <f aca="false">ROUND(MAX(I22*17%-I18,0)+I23*32%,0)</f>
+        <f aca="false">ROUND(MAX(I22*17%+I23*32%-I18,0),0)</f>
         <v>941</v>
       </c>
       <c r="J24" s="1" t="n">
-        <f aca="false">ROUND(MAX(J22*17%-J18,0)+J23*32%,0)</f>
+        <f aca="false">ROUND(MAX(J22*17%+J23*32%-J18,0),0)</f>
         <v>1771</v>
       </c>
       <c r="K24" s="1" t="n">
-        <f aca="false">ROUND(MAX(K22*17%-K18,0)+K23*32%,0)</f>
+        <f aca="false">ROUND(MAX(K22*17%+K23*32%-K18,0),0)</f>
         <v>2517</v>
       </c>
       <c r="L24" s="1" t="n">
-        <f aca="false">ROUND(MAX(L22*17%-L18,0)+L23*32%,0)</f>
+        <f aca="false">ROUND(MAX(L22*17%+L23*32%-L18,0),0)</f>
         <v>2517</v>
       </c>
       <c r="M24" s="1" t="n">
-        <f aca="false">ROUND(MAX(M22*17%-M18,0)+M23*32%,0)</f>
+        <f aca="false">ROUND(MAX(M22*17%+M23*32%-M18,0),0)</f>
         <v>2517</v>
       </c>
       <c r="N24" s="1" t="n">
-        <f aca="false">ROUND(MAX(N22*17%-N18,0)+N23*32%,0)</f>
+        <f aca="false">ROUND(MAX(N22*17%+N23*32%-N18,0),0)</f>
         <v>2517</v>
       </c>
       <c r="O24" s="1" t="n">
-        <f aca="false">ROUND(MAX(O22*17%-O18,0)+O23*32%,0)</f>
+        <f aca="false">ROUND(MAX(O22*17%+O23*32%-O18,0),0)</f>
         <v>2991</v>
       </c>
       <c r="P24" s="1" t="n">
-        <f aca="false">ROUND(MAX(P22*17%-P18,0)+P23*32%,0)</f>
-        <v>5539</v>
+        <f aca="false">ROUND(MAX(P22*17%+P23*32%-P18,0),0)</f>
+        <v>5114</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2062,7 +2032,7 @@
       </c>
       <c r="P27" s="9" t="n">
         <f aca="false">P2-P11-P14-P24-P25-P26</f>
-        <v>9765.78</v>
+        <v>10190.78</v>
       </c>
     </row>
   </sheetData>
@@ -2089,10 +2059,10 @@
       <selection pane="topRight" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="32.23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="32.22"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="51.93"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="3.08"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="12" min="5" style="1" width="11.52"/>
@@ -2150,40 +2120,40 @@
         <v>15</v>
       </c>
       <c r="E2" s="4" t="n">
-        <v>10000</v>
+        <v>3010</v>
       </c>
       <c r="F2" s="4" t="n">
-        <v>10000</v>
+        <v>4000</v>
       </c>
       <c r="G2" s="4" t="n">
-        <v>10000</v>
+        <v>5000</v>
       </c>
       <c r="H2" s="4" t="n">
-        <v>10000</v>
+        <v>8000</v>
       </c>
       <c r="I2" s="4" t="n">
         <v>10000</v>
       </c>
       <c r="J2" s="4" t="n">
-        <v>10000</v>
+        <v>15000</v>
       </c>
       <c r="K2" s="4" t="n">
-        <v>10000</v>
+        <v>20000</v>
       </c>
       <c r="L2" s="4" t="n">
-        <v>10000</v>
+        <v>20000</v>
       </c>
       <c r="M2" s="4" t="n">
-        <v>10000</v>
+        <v>20000</v>
       </c>
       <c r="N2" s="4" t="n">
-        <v>10000</v>
+        <v>20000</v>
       </c>
       <c r="O2" s="4" t="n">
-        <v>10000</v>
+        <v>20000</v>
       </c>
       <c r="P2" s="4" t="n">
-        <v>10000</v>
+        <v>20000</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2354,47 +2324,47 @@
       </c>
       <c r="F6" s="6" t="n">
         <f aca="false">E6-E7</f>
-        <v>147770</v>
+        <v>154760</v>
       </c>
       <c r="G6" s="6" t="n">
         <f aca="false">F6-F7</f>
-        <v>137770</v>
+        <v>150760</v>
       </c>
       <c r="H6" s="6" t="n">
         <f aca="false">G6-G7</f>
-        <v>127770</v>
+        <v>145760</v>
       </c>
       <c r="I6" s="6" t="n">
         <f aca="false">H6-H7</f>
-        <v>117770</v>
+        <v>137760</v>
       </c>
       <c r="J6" s="6" t="n">
         <f aca="false">I6-I7</f>
-        <v>107770</v>
+        <v>127760</v>
       </c>
       <c r="K6" s="6" t="n">
         <f aca="false">J6-J7</f>
-        <v>97770</v>
+        <v>112760</v>
       </c>
       <c r="L6" s="6" t="n">
         <f aca="false">K6-K7</f>
-        <v>87770</v>
+        <v>92760</v>
       </c>
       <c r="M6" s="6" t="n">
         <f aca="false">L6-L7</f>
-        <v>77770</v>
+        <v>72760</v>
       </c>
       <c r="N6" s="6" t="n">
         <f aca="false">M6-M7</f>
-        <v>67770</v>
+        <v>52760</v>
       </c>
       <c r="O6" s="6" t="n">
         <f aca="false">N6-N7</f>
-        <v>57770</v>
+        <v>32760</v>
       </c>
       <c r="P6" s="6" t="n">
         <f aca="false">O6-O7</f>
-        <v>47770</v>
+        <v>12760</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2412,19 +2382,19 @@
       </c>
       <c r="E7" s="6" t="n">
         <f aca="false">MIN(E2,E6)</f>
-        <v>10000</v>
+        <v>3010</v>
       </c>
       <c r="F7" s="6" t="n">
         <f aca="false">MIN(F2,F6)</f>
-        <v>10000</v>
+        <v>4000</v>
       </c>
       <c r="G7" s="6" t="n">
         <f aca="false">MIN(G2,G6)</f>
-        <v>10000</v>
+        <v>5000</v>
       </c>
       <c r="H7" s="6" t="n">
         <f aca="false">MIN(H2,H6)</f>
-        <v>10000</v>
+        <v>8000</v>
       </c>
       <c r="I7" s="6" t="n">
         <f aca="false">MIN(I2,I6)</f>
@@ -2432,31 +2402,31 @@
       </c>
       <c r="J7" s="6" t="n">
         <f aca="false">MIN(J2,J6)</f>
-        <v>10000</v>
+        <v>15000</v>
       </c>
       <c r="K7" s="6" t="n">
         <f aca="false">MIN(K2,K6)</f>
-        <v>10000</v>
+        <v>20000</v>
       </c>
       <c r="L7" s="6" t="n">
         <f aca="false">MIN(L2,L6)</f>
-        <v>10000</v>
+        <v>20000</v>
       </c>
       <c r="M7" s="6" t="n">
         <f aca="false">MIN(M2,M6)</f>
-        <v>10000</v>
+        <v>20000</v>
       </c>
       <c r="N7" s="6" t="n">
         <f aca="false">MIN(N2,N6)</f>
-        <v>10000</v>
+        <v>20000</v>
       </c>
       <c r="O7" s="6" t="n">
         <f aca="false">MIN(O2,O6)</f>
-        <v>10000</v>
+        <v>20000</v>
       </c>
       <c r="P7" s="6" t="n">
         <f aca="false">MIN(P2,P6)</f>
-        <v>10000</v>
+        <v>12760</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2474,19 +2444,19 @@
       </c>
       <c r="E8" s="6" t="n">
         <f aca="false">ROUND(E2*E3/100,2)</f>
-        <v>976</v>
+        <v>293.78</v>
       </c>
       <c r="F8" s="6" t="n">
         <f aca="false">ROUND(F2*F3/100,2)</f>
-        <v>976</v>
+        <v>390.4</v>
       </c>
       <c r="G8" s="6" t="n">
         <f aca="false">ROUND(G2*G3/100,2)</f>
-        <v>976</v>
+        <v>488</v>
       </c>
       <c r="H8" s="6" t="n">
         <f aca="false">ROUND(H2*H3/100,2)</f>
-        <v>976</v>
+        <v>780.8</v>
       </c>
       <c r="I8" s="6" t="n">
         <f aca="false">ROUND(I2*I3/100,2)</f>
@@ -2494,31 +2464,31 @@
       </c>
       <c r="J8" s="6" t="n">
         <f aca="false">ROUND(J2*J3/100,2)</f>
-        <v>976</v>
+        <v>1464</v>
       </c>
       <c r="K8" s="6" t="n">
         <f aca="false">ROUND(K2*K3/100,2)</f>
-        <v>976</v>
+        <v>1952</v>
       </c>
       <c r="L8" s="6" t="n">
         <f aca="false">ROUND(L2*L3/100,2)</f>
-        <v>976</v>
+        <v>1952</v>
       </c>
       <c r="M8" s="6" t="n">
         <f aca="false">ROUND(M2*M3/100,2)</f>
-        <v>976</v>
+        <v>1952</v>
       </c>
       <c r="N8" s="6" t="n">
         <f aca="false">ROUND(N2*N3/100,2)</f>
-        <v>976</v>
+        <v>1952</v>
       </c>
       <c r="O8" s="6" t="n">
         <f aca="false">ROUND(O2*O3/100,2)</f>
-        <v>976</v>
+        <v>1952</v>
       </c>
       <c r="P8" s="6" t="n">
         <f aca="false">ROUND(P2*P3/100,2)</f>
-        <v>976</v>
+        <v>1952</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2536,19 +2506,19 @@
       </c>
       <c r="E9" s="6" t="n">
         <f aca="false">ROUND(E2*E4/100,2)</f>
-        <v>150</v>
+        <v>45.15</v>
       </c>
       <c r="F9" s="6" t="n">
         <f aca="false">ROUND(F2*F4/100,2)</f>
-        <v>150</v>
+        <v>60</v>
       </c>
       <c r="G9" s="6" t="n">
         <f aca="false">ROUND(G2*G4/100,2)</f>
-        <v>150</v>
+        <v>75</v>
       </c>
       <c r="H9" s="6" t="n">
         <f aca="false">ROUND(H2*H4/100,2)</f>
-        <v>150</v>
+        <v>120</v>
       </c>
       <c r="I9" s="6" t="n">
         <f aca="false">ROUND(I2*I4/100,2)</f>
@@ -2556,31 +2526,31 @@
       </c>
       <c r="J9" s="6" t="n">
         <f aca="false">ROUND(J2*J4/100,2)</f>
-        <v>150</v>
+        <v>225</v>
       </c>
       <c r="K9" s="6" t="n">
         <f aca="false">ROUND(K2*K4/100,2)</f>
-        <v>150</v>
+        <v>300</v>
       </c>
       <c r="L9" s="6" t="n">
         <f aca="false">ROUND(L2*L4/100,2)</f>
-        <v>150</v>
+        <v>300</v>
       </c>
       <c r="M9" s="6" t="n">
         <f aca="false">ROUND(M2*M4/100,2)</f>
-        <v>150</v>
+        <v>300</v>
       </c>
       <c r="N9" s="6" t="n">
         <f aca="false">ROUND(N2*N4/100,2)</f>
-        <v>150</v>
+        <v>300</v>
       </c>
       <c r="O9" s="6" t="n">
         <f aca="false">ROUND(O2*O4/100,2)</f>
-        <v>150</v>
+        <v>300</v>
       </c>
       <c r="P9" s="6" t="n">
         <f aca="false">ROUND(P2*P4/100,2)</f>
-        <v>150</v>
+        <v>300</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2598,19 +2568,19 @@
       </c>
       <c r="E10" s="6" t="n">
         <f aca="false">ROUND(E2*E5/100,2)</f>
-        <v>245</v>
+        <v>73.75</v>
       </c>
       <c r="F10" s="6" t="n">
         <f aca="false">ROUND(F2*F5/100,2)</f>
-        <v>245</v>
+        <v>98</v>
       </c>
       <c r="G10" s="6" t="n">
         <f aca="false">ROUND(G2*G5/100,2)</f>
-        <v>245</v>
+        <v>122.5</v>
       </c>
       <c r="H10" s="6" t="n">
         <f aca="false">ROUND(H2*H5/100,2)</f>
-        <v>245</v>
+        <v>196</v>
       </c>
       <c r="I10" s="6" t="n">
         <f aca="false">ROUND(I2*I5/100,2)</f>
@@ -2618,31 +2588,31 @@
       </c>
       <c r="J10" s="6" t="n">
         <f aca="false">ROUND(J2*J5/100,2)</f>
-        <v>245</v>
+        <v>367.5</v>
       </c>
       <c r="K10" s="6" t="n">
         <f aca="false">ROUND(K2*K5/100,2)</f>
-        <v>245</v>
+        <v>490</v>
       </c>
       <c r="L10" s="6" t="n">
         <f aca="false">ROUND(L2*L5/100,2)</f>
-        <v>245</v>
+        <v>490</v>
       </c>
       <c r="M10" s="6" t="n">
         <f aca="false">ROUND(M2*M5/100,2)</f>
-        <v>245</v>
+        <v>490</v>
       </c>
       <c r="N10" s="6" t="n">
         <f aca="false">ROUND(N2*N5/100,2)</f>
-        <v>245</v>
+        <v>490</v>
       </c>
       <c r="O10" s="6" t="n">
         <f aca="false">ROUND(O2*O5/100,2)</f>
-        <v>245</v>
+        <v>490</v>
       </c>
       <c r="P10" s="6" t="n">
         <f aca="false">ROUND(P2*P5/100,2)</f>
-        <v>245</v>
+        <v>490</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2660,19 +2630,19 @@
       </c>
       <c r="E11" s="1" t="n">
         <f aca="false">E8+E9+E10</f>
-        <v>1371</v>
+        <v>412.68</v>
       </c>
       <c r="F11" s="1" t="n">
         <f aca="false">F8+F9+F10</f>
-        <v>1371</v>
+        <v>548.4</v>
       </c>
       <c r="G11" s="1" t="n">
         <f aca="false">G8+G9+G10</f>
-        <v>1371</v>
+        <v>685.5</v>
       </c>
       <c r="H11" s="1" t="n">
         <f aca="false">H8+H9+H10</f>
-        <v>1371</v>
+        <v>1096.8</v>
       </c>
       <c r="I11" s="1" t="n">
         <f aca="false">I8+I9+I10</f>
@@ -2680,31 +2650,31 @@
       </c>
       <c r="J11" s="1" t="n">
         <f aca="false">J8+J9+J10</f>
-        <v>1371</v>
+        <v>2056.5</v>
       </c>
       <c r="K11" s="1" t="n">
         <f aca="false">K8+K9+K10</f>
-        <v>1371</v>
+        <v>2742</v>
       </c>
       <c r="L11" s="1" t="n">
         <f aca="false">L8+L9+L10</f>
-        <v>1371</v>
+        <v>2742</v>
       </c>
       <c r="M11" s="1" t="n">
         <f aca="false">M8+M9+M10</f>
-        <v>1371</v>
+        <v>2742</v>
       </c>
       <c r="N11" s="1" t="n">
         <f aca="false">N8+N9+N10</f>
-        <v>1371</v>
+        <v>2742</v>
       </c>
       <c r="O11" s="1" t="n">
         <f aca="false">O8+O9+O10</f>
-        <v>1371</v>
+        <v>2742</v>
       </c>
       <c r="P11" s="1" t="n">
         <f aca="false">P8+P9+P10</f>
-        <v>1371</v>
+        <v>2742</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2722,19 +2692,19 @@
       </c>
       <c r="E12" s="1" t="n">
         <f aca="false">E2-E11</f>
-        <v>8629</v>
+        <v>2597.32</v>
       </c>
       <c r="F12" s="1" t="n">
         <f aca="false">F2-F11</f>
-        <v>8629</v>
+        <v>3451.6</v>
       </c>
       <c r="G12" s="1" t="n">
         <f aca="false">G2-G11</f>
-        <v>8629</v>
+        <v>4314.5</v>
       </c>
       <c r="H12" s="1" t="n">
         <f aca="false">H2-H11</f>
-        <v>8629</v>
+        <v>6903.2</v>
       </c>
       <c r="I12" s="1" t="n">
         <f aca="false">I2-I11</f>
@@ -2742,31 +2712,31 @@
       </c>
       <c r="J12" s="1" t="n">
         <f aca="false">J2-J11</f>
-        <v>8629</v>
+        <v>12943.5</v>
       </c>
       <c r="K12" s="1" t="n">
         <f aca="false">K2-K11</f>
-        <v>8629</v>
+        <v>17258</v>
       </c>
       <c r="L12" s="1" t="n">
         <f aca="false">L2-L11</f>
-        <v>8629</v>
+        <v>17258</v>
       </c>
       <c r="M12" s="1" t="n">
         <f aca="false">M2-M11</f>
-        <v>8629</v>
+        <v>17258</v>
       </c>
       <c r="N12" s="1" t="n">
         <f aca="false">N2-N11</f>
-        <v>8629</v>
+        <v>17258</v>
       </c>
       <c r="O12" s="1" t="n">
         <f aca="false">O2-O11</f>
-        <v>8629</v>
+        <v>17258</v>
       </c>
       <c r="P12" s="1" t="n">
         <f aca="false">P2-P11</f>
-        <v>8629</v>
+        <v>17258</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2784,19 +2754,19 @@
       </c>
       <c r="E13" s="1" t="n">
         <f aca="false">ROUND(E12*7.75%,2)</f>
-        <v>668.75</v>
+        <v>201.29</v>
       </c>
       <c r="F13" s="1" t="n">
         <f aca="false">ROUND(F12*7.75%,2)</f>
-        <v>668.75</v>
+        <v>267.5</v>
       </c>
       <c r="G13" s="1" t="n">
         <f aca="false">ROUND(G12*7.75%,2)</f>
-        <v>668.75</v>
+        <v>334.37</v>
       </c>
       <c r="H13" s="1" t="n">
         <f aca="false">ROUND(H12*7.75%,2)</f>
-        <v>668.75</v>
+        <v>535</v>
       </c>
       <c r="I13" s="1" t="n">
         <f aca="false">ROUND(I12*7.75%,2)</f>
@@ -2804,31 +2774,31 @@
       </c>
       <c r="J13" s="1" t="n">
         <f aca="false">ROUND(J12*7.75%,2)</f>
-        <v>668.75</v>
+        <v>1003.12</v>
       </c>
       <c r="K13" s="1" t="n">
         <f aca="false">ROUND(K12*7.75%,2)</f>
-        <v>668.75</v>
+        <v>1337.5</v>
       </c>
       <c r="L13" s="1" t="n">
         <f aca="false">ROUND(L12*7.75%,2)</f>
-        <v>668.75</v>
+        <v>1337.5</v>
       </c>
       <c r="M13" s="1" t="n">
         <f aca="false">ROUND(M12*7.75%,2)</f>
-        <v>668.75</v>
+        <v>1337.5</v>
       </c>
       <c r="N13" s="1" t="n">
         <f aca="false">ROUND(N12*7.75%,2)</f>
-        <v>668.75</v>
+        <v>1337.5</v>
       </c>
       <c r="O13" s="1" t="n">
         <f aca="false">ROUND(O12*7.75%,2)</f>
-        <v>668.75</v>
+        <v>1337.5</v>
       </c>
       <c r="P13" s="1" t="n">
         <f aca="false">ROUND(P12*7.75%,2)</f>
-        <v>668.75</v>
+        <v>1337.5</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2846,19 +2816,19 @@
       </c>
       <c r="E14" s="1" t="n">
         <f aca="false">ROUND(E12*9%,2)</f>
-        <v>776.61</v>
+        <v>233.76</v>
       </c>
       <c r="F14" s="1" t="n">
         <f aca="false">ROUND(F12*9%,2)</f>
-        <v>776.61</v>
+        <v>310.64</v>
       </c>
       <c r="G14" s="1" t="n">
         <f aca="false">ROUND(G12*9%,2)</f>
-        <v>776.61</v>
+        <v>388.31</v>
       </c>
       <c r="H14" s="1" t="n">
         <f aca="false">ROUND(H12*9%,2)</f>
-        <v>776.61</v>
+        <v>621.29</v>
       </c>
       <c r="I14" s="1" t="n">
         <f aca="false">ROUND(I12*9%,2)</f>
@@ -2866,31 +2836,31 @@
       </c>
       <c r="J14" s="1" t="n">
         <f aca="false">ROUND(J12*9%,2)</f>
-        <v>776.61</v>
+        <v>1164.92</v>
       </c>
       <c r="K14" s="1" t="n">
         <f aca="false">ROUND(K12*9%,2)</f>
-        <v>776.61</v>
+        <v>1553.22</v>
       </c>
       <c r="L14" s="1" t="n">
         <f aca="false">ROUND(L12*9%,2)</f>
-        <v>776.61</v>
+        <v>1553.22</v>
       </c>
       <c r="M14" s="1" t="n">
         <f aca="false">ROUND(M12*9%,2)</f>
-        <v>776.61</v>
+        <v>1553.22</v>
       </c>
       <c r="N14" s="1" t="n">
         <f aca="false">ROUND(N12*9%,2)</f>
-        <v>776.61</v>
+        <v>1553.22</v>
       </c>
       <c r="O14" s="1" t="n">
         <f aca="false">ROUND(O12*9%,2)</f>
-        <v>776.61</v>
+        <v>1553.22</v>
       </c>
       <c r="P14" s="1" t="n">
         <f aca="false">ROUND(P12*9%,2)</f>
-        <v>776.61</v>
+        <v>1553.22</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3008,19 +2978,19 @@
       </c>
       <c r="E17" s="1" t="n">
         <f aca="false">IF(E16&gt;0,ROUND(E2*1.5%,2),0)</f>
-        <v>150</v>
+        <v>45.15</v>
       </c>
       <c r="F17" s="1" t="n">
         <f aca="false">IF(F16&gt;0,ROUND(F2*1.5%,2),0)</f>
-        <v>150</v>
+        <v>60</v>
       </c>
       <c r="G17" s="1" t="n">
         <f aca="false">IF(G16&gt;0,ROUND(G2*1.5%,2),0)</f>
-        <v>150</v>
+        <v>75</v>
       </c>
       <c r="H17" s="1" t="n">
         <f aca="false">IF(H16&gt;0,ROUND(H2*1.5%,2),0)</f>
-        <v>150</v>
+        <v>120</v>
       </c>
       <c r="I17" s="1" t="n">
         <f aca="false">IF(I16&gt;0,ROUND(I2*1.5%,2),0)</f>
@@ -3028,31 +2998,31 @@
       </c>
       <c r="J17" s="1" t="n">
         <f aca="false">IF(J16&gt;0,ROUND(J2*1.5%,2),0)</f>
-        <v>150</v>
+        <v>225</v>
       </c>
       <c r="K17" s="1" t="n">
         <f aca="false">IF(K16&gt;0,ROUND(K2*1.5%,2),0)</f>
-        <v>150</v>
+        <v>300</v>
       </c>
       <c r="L17" s="1" t="n">
         <f aca="false">IF(L16&gt;0,ROUND(L2*1.5%,2),0)</f>
-        <v>150</v>
+        <v>300</v>
       </c>
       <c r="M17" s="1" t="n">
         <f aca="false">IF(M16&gt;0,ROUND(M2*1.5%,2),0)</f>
-        <v>150</v>
+        <v>300</v>
       </c>
       <c r="N17" s="1" t="n">
         <f aca="false">IF(N16&gt;0,ROUND(N2*1.5%,2),0)</f>
-        <v>150</v>
+        <v>300</v>
       </c>
       <c r="O17" s="1" t="n">
         <f aca="false">IF(O16&gt;0,ROUND(O2*1.5%,2),0)</f>
-        <v>150</v>
+        <v>300</v>
       </c>
       <c r="P17" s="1" t="n">
         <f aca="false">IF(P16&gt;0,ROUND(P2*1.5%,2),0)</f>
-        <v>150</v>
+        <v>300</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3105,11 +3075,11 @@
       </c>
       <c r="N18" s="6" t="n">
         <f aca="false">IF(N20&gt;0,M18,0)</f>
-        <v>43.76</v>
+        <v>0</v>
       </c>
       <c r="O18" s="6" t="n">
         <f aca="false">IF(O20&gt;0,N18,0)</f>
-        <v>43.76</v>
+        <v>0</v>
       </c>
       <c r="P18" s="6" t="n">
         <f aca="false">IF(P20&gt;0,O18,0)</f>
@@ -3184,43 +3154,43 @@
       </c>
       <c r="F20" s="6" t="n">
         <f aca="false">E20-E22</f>
-        <v>76999</v>
+        <v>83136</v>
       </c>
       <c r="G20" s="6" t="n">
         <f aca="false">F20-F22</f>
-        <v>68470</v>
+        <v>79874</v>
       </c>
       <c r="H20" s="6" t="n">
         <f aca="false">G20-G22</f>
-        <v>59941</v>
+        <v>75734</v>
       </c>
       <c r="I20" s="6" t="n">
         <f aca="false">H20-H22</f>
-        <v>51412</v>
+        <v>68961</v>
       </c>
       <c r="J20" s="6" t="n">
         <f aca="false">I20-I22</f>
-        <v>42883</v>
+        <v>60432</v>
       </c>
       <c r="K20" s="6" t="n">
         <f aca="false">J20-J22</f>
-        <v>34354</v>
+        <v>47513</v>
       </c>
       <c r="L20" s="6" t="n">
         <f aca="false">K20-K22</f>
-        <v>25825</v>
+        <v>30205</v>
       </c>
       <c r="M20" s="6" t="n">
         <f aca="false">L20-L22</f>
-        <v>17296</v>
+        <v>12897</v>
       </c>
       <c r="N20" s="6" t="n">
         <f aca="false">M20-M22</f>
-        <v>8767</v>
+        <v>0</v>
       </c>
       <c r="O20" s="6" t="n">
         <f aca="false">N20-N22</f>
-        <v>238</v>
+        <v>0</v>
       </c>
       <c r="P20" s="6" t="n">
         <f aca="false">O20-O22</f>
@@ -3242,19 +3212,19 @@
       </c>
       <c r="E21" s="1" t="n">
         <f aca="false">ROUND(MAX(E2+E17-E11-E15-E19,0),0)</f>
-        <v>8529</v>
+        <v>2392</v>
       </c>
       <c r="F21" s="1" t="n">
         <f aca="false">ROUND(MAX(F2+F17-F11-F15-F19,0),0)</f>
-        <v>8529</v>
+        <v>3262</v>
       </c>
       <c r="G21" s="1" t="n">
         <f aca="false">ROUND(MAX(G2+G17-G11-G15-G19,0),0)</f>
-        <v>8529</v>
+        <v>4140</v>
       </c>
       <c r="H21" s="1" t="n">
         <f aca="false">ROUND(MAX(H2+H17-H11-H15-H19,0),0)</f>
-        <v>8529</v>
+        <v>6773</v>
       </c>
       <c r="I21" s="1" t="n">
         <f aca="false">ROUND(MAX(I2+I17-I11-I15-I19,0),0)</f>
@@ -3262,31 +3232,31 @@
       </c>
       <c r="J21" s="1" t="n">
         <f aca="false">ROUND(MAX(J2+J17-J11-J15-J19,0),0)</f>
-        <v>8529</v>
+        <v>12919</v>
       </c>
       <c r="K21" s="1" t="n">
         <f aca="false">ROUND(MAX(K2+K17-K11-K15-K19,0),0)</f>
-        <v>8529</v>
+        <v>17308</v>
       </c>
       <c r="L21" s="1" t="n">
         <f aca="false">ROUND(MAX(L2+L17-L11-L15-L19,0),0)</f>
-        <v>8529</v>
+        <v>17308</v>
       </c>
       <c r="M21" s="1" t="n">
         <f aca="false">ROUND(MAX(M2+M17-M11-M15-M19,0),0)</f>
-        <v>8529</v>
+        <v>17308</v>
       </c>
       <c r="N21" s="1" t="n">
         <f aca="false">ROUND(MAX(N2+N17-N11-N15-N19,0),0)</f>
-        <v>8529</v>
+        <v>17308</v>
       </c>
       <c r="O21" s="1" t="n">
         <f aca="false">ROUND(MAX(O2+O17-O11-O15-O19,0),0)</f>
-        <v>8529</v>
+        <v>17308</v>
       </c>
       <c r="P21" s="1" t="n">
         <f aca="false">ROUND(MAX(P2+P17-P11-P15-P19,0),0)</f>
-        <v>8529</v>
+        <v>17308</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3304,19 +3274,19 @@
       </c>
       <c r="E22" s="6" t="n">
         <f aca="false">MIN(E21,E20)</f>
-        <v>8529</v>
+        <v>2392</v>
       </c>
       <c r="F22" s="6" t="n">
         <f aca="false">MIN(F21,F20)</f>
-        <v>8529</v>
+        <v>3262</v>
       </c>
       <c r="G22" s="6" t="n">
         <f aca="false">MIN(G21,G20)</f>
-        <v>8529</v>
+        <v>4140</v>
       </c>
       <c r="H22" s="6" t="n">
         <f aca="false">MIN(H21,H20)</f>
-        <v>8529</v>
+        <v>6773</v>
       </c>
       <c r="I22" s="6" t="n">
         <f aca="false">MIN(I21,I20)</f>
@@ -3324,27 +3294,27 @@
       </c>
       <c r="J22" s="6" t="n">
         <f aca="false">MIN(J21,J20)</f>
-        <v>8529</v>
+        <v>12919</v>
       </c>
       <c r="K22" s="6" t="n">
         <f aca="false">MIN(K21,K20)</f>
-        <v>8529</v>
+        <v>17308</v>
       </c>
       <c r="L22" s="6" t="n">
         <f aca="false">MIN(L21,L20)</f>
-        <v>8529</v>
+        <v>17308</v>
       </c>
       <c r="M22" s="6" t="n">
         <f aca="false">MIN(M21,M20)</f>
-        <v>8529</v>
+        <v>12897</v>
       </c>
       <c r="N22" s="6" t="n">
         <f aca="false">MIN(N21,N20)</f>
-        <v>8529</v>
+        <v>0</v>
       </c>
       <c r="O22" s="6" t="n">
         <f aca="false">MIN(O21,O20)</f>
-        <v>238</v>
+        <v>0</v>
       </c>
       <c r="P22" s="6" t="n">
         <f aca="false">MIN(P21,P20)</f>
@@ -3398,19 +3368,19 @@
       </c>
       <c r="M23" s="6" t="n">
         <f aca="false">M21-M22</f>
-        <v>0</v>
+        <v>4411</v>
       </c>
       <c r="N23" s="6" t="n">
         <f aca="false">N21-N22</f>
-        <v>0</v>
+        <v>17308</v>
       </c>
       <c r="O23" s="6" t="n">
         <f aca="false">O21-O22</f>
-        <v>8291</v>
+        <v>17308</v>
       </c>
       <c r="P23" s="6" t="n">
         <f aca="false">P21-P22</f>
-        <v>8529</v>
+        <v>17308</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3427,52 +3397,52 @@
         <v>15</v>
       </c>
       <c r="E24" s="1" t="n">
-        <f aca="false">ROUND(MAX(E22*17%-E18,0)+E23*32%-E13,0)</f>
+        <f aca="false">ROUND(MAX(E22*17%+E23*32%-E18-E13,0),0)</f>
+        <v>162</v>
+      </c>
+      <c r="F24" s="1" t="n">
+        <f aca="false">ROUND(MAX(F22*17%+F23*32%-F18-F13,0),0)</f>
+        <v>243</v>
+      </c>
+      <c r="G24" s="1" t="n">
+        <f aca="false">ROUND(MAX(G22*17%+G23*32%-G18-G13,0),0)</f>
+        <v>326</v>
+      </c>
+      <c r="H24" s="1" t="n">
+        <f aca="false">ROUND(MAX(H22*17%+H23*32%-H18-H13,0),0)</f>
+        <v>573</v>
+      </c>
+      <c r="I24" s="1" t="n">
+        <f aca="false">ROUND(MAX(I22*17%+I23*32%-I18-I13,0),0)</f>
         <v>737</v>
       </c>
-      <c r="F24" s="1" t="n">
-        <f aca="false">ROUND(MAX(F22*17%-F18,0)+F23*32%-F13,0)</f>
-        <v>737</v>
-      </c>
-      <c r="G24" s="1" t="n">
-        <f aca="false">ROUND(MAX(G22*17%-G18,0)+G23*32%-G13,0)</f>
-        <v>737</v>
-      </c>
-      <c r="H24" s="1" t="n">
-        <f aca="false">ROUND(MAX(H22*17%-H18,0)+H23*32%-H13,0)</f>
-        <v>737</v>
-      </c>
-      <c r="I24" s="1" t="n">
-        <f aca="false">ROUND(MAX(I22*17%-I18,0)+I23*32%-I13,0)</f>
-        <v>737</v>
-      </c>
       <c r="J24" s="1" t="n">
-        <f aca="false">ROUND(MAX(J22*17%-J18,0)+J23*32%-J13,0)</f>
-        <v>737</v>
+        <f aca="false">ROUND(MAX(J22*17%+J23*32%-J18-J13,0),0)</f>
+        <v>1149</v>
       </c>
       <c r="K24" s="1" t="n">
-        <f aca="false">ROUND(MAX(K22*17%-K18,0)+K23*32%-K13,0)</f>
-        <v>737</v>
+        <f aca="false">ROUND(MAX(K22*17%+K23*32%-K18-K13,0),0)</f>
+        <v>1561</v>
       </c>
       <c r="L24" s="1" t="n">
-        <f aca="false">ROUND(MAX(L22*17%-L18,0)+L23*32%-L13,0)</f>
-        <v>737</v>
+        <f aca="false">ROUND(MAX(L22*17%+L23*32%-L18-L13,0),0)</f>
+        <v>1561</v>
       </c>
       <c r="M24" s="1" t="n">
-        <f aca="false">ROUND(MAX(M22*17%-M18,0)+M23*32%-M13,0)</f>
-        <v>737</v>
+        <f aca="false">ROUND(MAX(M22*17%+M23*32%-M18-M13,0),0)</f>
+        <v>2223</v>
       </c>
       <c r="N24" s="1" t="n">
-        <f aca="false">ROUND(MAX(N22*17%-N18,0)+N23*32%-N13,0)</f>
-        <v>737</v>
+        <f aca="false">ROUND(MAX(N22*17%+N23*32%-N18-N13,0),0)</f>
+        <v>4201</v>
       </c>
       <c r="O24" s="1" t="n">
-        <f aca="false">ROUND(MAX(O22*17%-O18,0)+O23*32%-O13,0)</f>
-        <v>1984</v>
+        <f aca="false">ROUND(MAX(O22*17%+O23*32%-O18-O13,0),0)</f>
+        <v>4201</v>
       </c>
       <c r="P24" s="1" t="n">
         <f aca="false">ROUND(MAX(P22*17%-P18,0)+P23*32%-P13,0)</f>
-        <v>2061</v>
+        <v>4201</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3490,19 +3460,19 @@
       </c>
       <c r="E25" s="1" t="n">
         <f aca="false">ROUND(E2*E16/100,2)</f>
-        <v>200</v>
+        <v>60.2</v>
       </c>
       <c r="F25" s="1" t="n">
         <f aca="false">ROUND(F2*F16/100,2)</f>
-        <v>200</v>
+        <v>80</v>
       </c>
       <c r="G25" s="1" t="n">
         <f aca="false">ROUND(G2*G16/100,2)</f>
-        <v>200</v>
+        <v>100</v>
       </c>
       <c r="H25" s="1" t="n">
         <f aca="false">ROUND(H2*H16/100,2)</f>
-        <v>200</v>
+        <v>160</v>
       </c>
       <c r="I25" s="1" t="n">
         <f aca="false">ROUND(I2*I16/100,2)</f>
@@ -3510,31 +3480,31 @@
       </c>
       <c r="J25" s="1" t="n">
         <f aca="false">ROUND(J2*J16/100,2)</f>
-        <v>200</v>
+        <v>300</v>
       </c>
       <c r="K25" s="1" t="n">
         <f aca="false">ROUND(K2*K16/100,2)</f>
-        <v>200</v>
+        <v>400</v>
       </c>
       <c r="L25" s="1" t="n">
         <f aca="false">ROUND(L2*L16/100,2)</f>
-        <v>200</v>
+        <v>400</v>
       </c>
       <c r="M25" s="1" t="n">
         <f aca="false">ROUND(M2*M16/100,2)</f>
-        <v>200</v>
+        <v>400</v>
       </c>
       <c r="N25" s="1" t="n">
         <f aca="false">ROUND(N2*N16/100,2)</f>
-        <v>200</v>
+        <v>400</v>
       </c>
       <c r="O25" s="1" t="n">
         <f aca="false">ROUND(O2*O16/100,2)</f>
-        <v>200</v>
+        <v>400</v>
       </c>
       <c r="P25" s="1" t="n">
         <f aca="false">ROUND(P2*P16/100,2)</f>
-        <v>200</v>
+        <v>400</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3600,19 +3570,19 @@
       </c>
       <c r="E27" s="9" t="n">
         <f aca="false">E2-E11-E14-E24-E25-E26</f>
-        <v>6915.39</v>
+        <v>2141.36</v>
       </c>
       <c r="F27" s="9" t="n">
         <f aca="false">F2-F11-F14-F24-F25-F26</f>
-        <v>6915.39</v>
+        <v>2817.96</v>
       </c>
       <c r="G27" s="9" t="n">
         <f aca="false">G2-G11-G14-G24-G25-G26</f>
-        <v>6915.39</v>
+        <v>3500.19</v>
       </c>
       <c r="H27" s="9" t="n">
         <f aca="false">H2-H11-H14-H24-H25-H26</f>
-        <v>6915.39</v>
+        <v>5548.91</v>
       </c>
       <c r="I27" s="9" t="n">
         <f aca="false">I2-I11-I14-I24-I25-I26</f>
@@ -3620,31 +3590,31 @@
       </c>
       <c r="J27" s="9" t="n">
         <f aca="false">J2-J11-J14-J24-J25-J26</f>
-        <v>6915.39</v>
+        <v>10329.58</v>
       </c>
       <c r="K27" s="9" t="n">
         <f aca="false">K2-K11-K14-K24-K25-K26</f>
-        <v>6915.39</v>
+        <v>13743.78</v>
       </c>
       <c r="L27" s="9" t="n">
         <f aca="false">L2-L11-L14-L24-L25-L26</f>
-        <v>6915.39</v>
+        <v>13743.78</v>
       </c>
       <c r="M27" s="9" t="n">
         <f aca="false">M2-M11-M14-M24-M25-M26</f>
-        <v>6915.39</v>
+        <v>13081.78</v>
       </c>
       <c r="N27" s="9" t="n">
         <f aca="false">N2-N11-N14-N24-N25-N26</f>
-        <v>6915.39</v>
+        <v>11103.78</v>
       </c>
       <c r="O27" s="9" t="n">
         <f aca="false">O2-O11-O14-O24-O25-O26</f>
-        <v>5668.39</v>
+        <v>11103.78</v>
       </c>
       <c r="P27" s="9" t="n">
         <f aca="false">P2-P11-P14-P24-P25-P26</f>
-        <v>5591.39</v>
+        <v>11103.78</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Pokazuj średnią netto z całego roku
</commit_message>
<xml_diff>
--- a/polski-lad-netto.xlsx
+++ b/polski-lad-netto.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="103">
   <si>
     <t xml:space="preserve">sty</t>
   </si>
@@ -294,6 +294,15 @@
   </si>
   <si>
     <t xml:space="preserve">Brutto-Zus-SklZdr-ZalPod-PPK-Potr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NettoSr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">netto srednio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Suma(Netto)/12</t>
   </si>
   <si>
     <t xml:space="preserve">157.770zł@sty, zmniejsza się o PodstEmerRent</t>
@@ -469,7 +478,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:P27"/>
+  <dimension ref="A1:P28"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="0" topLeftCell="B1" activePane="topRight" state="frozen"/>
@@ -477,7 +486,7 @@
       <selection pane="topRight" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="32.22"/>
@@ -2033,6 +2042,24 @@
       <c r="P27" s="9" t="n">
         <f aca="false">P2-P11-P14-P24-P25-P26</f>
         <v>10190.78</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="B28" s="0" t="s">
+        <v>92</v>
+      </c>
+      <c r="C28" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="D28" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="E28" s="1" t="n">
+        <f aca="false">ROUND(SUM(E27:P27)/12,2)</f>
+        <v>8700.42</v>
       </c>
     </row>
   </sheetData>
@@ -2051,7 +2078,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:P27"/>
+  <dimension ref="A1:P28"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="0" topLeftCell="B1" activePane="topRight" state="frozen"/>
@@ -2059,7 +2086,7 @@
       <selection pane="topRight" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="32.22"/>
@@ -2314,7 +2341,7 @@
         <v>27</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="D6" s="5" t="s">
         <v>15</v>
@@ -2741,13 +2768,13 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="B13" s="0" t="s">
         <v>48</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="D13" s="5" t="s">
         <v>15</v>
@@ -2871,7 +2898,7 @@
         <v>54</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="D15" s="5" t="s">
         <v>15</v>
@@ -3027,13 +3054,13 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="D18" s="5" t="s">
         <v>15</v>
@@ -3144,7 +3171,7 @@
         <v>69</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="D20" s="5" t="s">
         <v>15</v>
@@ -3391,7 +3418,7 @@
         <v>81</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="D24" s="5" t="s">
         <v>15</v>
@@ -3615,6 +3642,24 @@
       <c r="P27" s="9" t="n">
         <f aca="false">P2-P11-P14-P24-P25-P26</f>
         <v>11103.78</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="B28" s="0" t="s">
+        <v>92</v>
+      </c>
+      <c r="C28" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="D28" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="E28" s="1" t="n">
+        <f aca="false">ROUND(SUM(E27:P27)/12,2)</f>
+        <v>8761.17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix #1 ZusEmer ZusRent w 2021 wyliczany z PodstEmerRent
</commit_message>
<xml_diff>
--- a/polski-lad-netto.xlsx
+++ b/polski-lad-netto.xlsx
@@ -21,12 +21,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="114">
   <si>
     <t xml:space="preserve">Wersja</t>
   </si>
   <si>
-    <t xml:space="preserve">1.0.0</t>
+    <t xml:space="preserve">1.0.1</t>
   </si>
   <si>
     <t xml:space="preserve">https://github.com/tometzky/polski-lad-netto</t>
@@ -89,23 +89,7 @@
     <t xml:space="preserve">pensja brutto ze świadczeniami niep.</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Brutto+</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">BruttoNiep</t>
-    </r>
+    <t xml:space="preserve">Brutto+BruttoNiep</t>
   </si>
   <si>
     <t xml:space="preserve">ProcZusEmer</t>
@@ -348,80 +332,16 @@
     <t xml:space="preserve">min(PostBrutto, LimEmerRent)</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Post</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Brutto*ProcZusEmer/100</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Post</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Brutto*ProcZusRent/100</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Post</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Brutto*ProcZusChor/100</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Post</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Brutto-Zus</t>
-    </r>
+    <t xml:space="preserve">PostBrutto*ProcZusEmer/100</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PostBrutto*ProcZusRent/100</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PostBrutto*ProcZusChor/100</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PostBrutto-Zus</t>
   </si>
   <si>
     <t xml:space="preserve">SklZdrDoOdl</t>
@@ -443,25 +363,6 @@
   </si>
   <si>
     <t xml:space="preserve">PodstOp*ProcPod/100%-UlgZmZal-SklZdrDoOdl</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Podst</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Brutto*ProcPPK/100</t>
-    </r>
   </si>
 </sst>
 </file>
@@ -473,7 +374,7 @@
     <numFmt numFmtId="165" formatCode="#,##0.00"/>
     <numFmt numFmtId="166" formatCode="0.00%"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -508,11 +409,6 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -564,7 +460,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="11">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -609,14 +505,6 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -642,7 +530,7 @@
       <selection pane="topRight" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="32.22"/>
@@ -2360,7 +2248,7 @@
       <selection pane="topRight" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="32.22"/>
@@ -2843,59 +2731,59 @@
       <c r="B10" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="C10" s="11" t="s">
+      <c r="C10" s="7" t="s">
         <v>103</v>
       </c>
       <c r="D10" s="7" t="s">
         <v>17</v>
       </c>
       <c r="E10" s="6" t="n">
-        <f aca="false">ROUND(E4*E5/100,2)</f>
+        <f aca="false">ROUND(E9*E5/100,2)</f>
         <v>293.78</v>
       </c>
       <c r="F10" s="6" t="n">
-        <f aca="false">ROUND(F4*F5/100,2)</f>
+        <f aca="false">ROUND(F9*F5/100,2)</f>
         <v>390.4</v>
       </c>
       <c r="G10" s="6" t="n">
-        <f aca="false">ROUND(G4*G5/100,2)</f>
+        <f aca="false">ROUND(G9*G5/100,2)</f>
         <v>488</v>
       </c>
       <c r="H10" s="6" t="n">
-        <f aca="false">ROUND(H4*H5/100,2)</f>
+        <f aca="false">ROUND(H9*H5/100,2)</f>
         <v>780.8</v>
       </c>
       <c r="I10" s="6" t="n">
-        <f aca="false">ROUND(I4*I5/100,2)</f>
+        <f aca="false">ROUND(I9*I5/100,2)</f>
         <v>976</v>
       </c>
       <c r="J10" s="6" t="n">
-        <f aca="false">ROUND(J4*J5/100,2)</f>
+        <f aca="false">ROUND(J9*J5/100,2)</f>
         <v>1464</v>
       </c>
       <c r="K10" s="6" t="n">
-        <f aca="false">ROUND(K4*K5/100,2)</f>
+        <f aca="false">ROUND(K9*K5/100,2)</f>
         <v>1952</v>
       </c>
       <c r="L10" s="6" t="n">
-        <f aca="false">ROUND(L4*L5/100,2)</f>
+        <f aca="false">ROUND(L9*L5/100,2)</f>
         <v>1952</v>
       </c>
       <c r="M10" s="6" t="n">
-        <f aca="false">ROUND(M4*M5/100,2)</f>
+        <f aca="false">ROUND(M9*M5/100,2)</f>
         <v>1952</v>
       </c>
       <c r="N10" s="6" t="n">
-        <f aca="false">ROUND(N4*N5/100,2)</f>
+        <f aca="false">ROUND(N9*N5/100,2)</f>
         <v>1952</v>
       </c>
       <c r="O10" s="6" t="n">
-        <f aca="false">ROUND(O4*O5/100,2)</f>
+        <f aca="false">ROUND(O9*O5/100,2)</f>
         <v>1952</v>
       </c>
       <c r="P10" s="6" t="n">
-        <f aca="false">ROUND(P4*P5/100,2)</f>
-        <v>1952</v>
+        <f aca="false">ROUND(P9*P5/100,2)</f>
+        <v>1245.38</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2905,59 +2793,59 @@
       <c r="B11" s="0" t="s">
         <v>43</v>
       </c>
-      <c r="C11" s="11" t="s">
+      <c r="C11" s="7" t="s">
         <v>104</v>
       </c>
       <c r="D11" s="7" t="s">
         <v>17</v>
       </c>
       <c r="E11" s="6" t="n">
-        <f aca="false">ROUND(E4*E6/100,2)</f>
+        <f aca="false">ROUND(E9*E6/100,2)</f>
         <v>45.15</v>
       </c>
       <c r="F11" s="6" t="n">
-        <f aca="false">ROUND(F4*F6/100,2)</f>
+        <f aca="false">ROUND(F9*F6/100,2)</f>
         <v>60</v>
       </c>
       <c r="G11" s="6" t="n">
-        <f aca="false">ROUND(G4*G6/100,2)</f>
+        <f aca="false">ROUND(G9*G6/100,2)</f>
         <v>75</v>
       </c>
       <c r="H11" s="6" t="n">
-        <f aca="false">ROUND(H4*H6/100,2)</f>
+        <f aca="false">ROUND(H9*H6/100,2)</f>
         <v>120</v>
       </c>
       <c r="I11" s="6" t="n">
-        <f aca="false">ROUND(I4*I6/100,2)</f>
+        <f aca="false">ROUND(I9*I6/100,2)</f>
         <v>150</v>
       </c>
       <c r="J11" s="6" t="n">
-        <f aca="false">ROUND(J4*J6/100,2)</f>
+        <f aca="false">ROUND(J9*J6/100,2)</f>
         <v>225</v>
       </c>
       <c r="K11" s="6" t="n">
-        <f aca="false">ROUND(K4*K6/100,2)</f>
+        <f aca="false">ROUND(K9*K6/100,2)</f>
         <v>300</v>
       </c>
       <c r="L11" s="6" t="n">
-        <f aca="false">ROUND(L4*L6/100,2)</f>
+        <f aca="false">ROUND(L9*L6/100,2)</f>
         <v>300</v>
       </c>
       <c r="M11" s="6" t="n">
-        <f aca="false">ROUND(M4*M6/100,2)</f>
+        <f aca="false">ROUND(M9*M6/100,2)</f>
         <v>300</v>
       </c>
       <c r="N11" s="6" t="n">
-        <f aca="false">ROUND(N4*N6/100,2)</f>
+        <f aca="false">ROUND(N9*N6/100,2)</f>
         <v>300</v>
       </c>
       <c r="O11" s="6" t="n">
-        <f aca="false">ROUND(O4*O6/100,2)</f>
+        <f aca="false">ROUND(O9*O6/100,2)</f>
         <v>300</v>
       </c>
       <c r="P11" s="6" t="n">
-        <f aca="false">ROUND(P4*P6/100,2)</f>
-        <v>300</v>
+        <f aca="false">ROUND(P9*P6/100,2)</f>
+        <v>191.4</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2967,7 +2855,7 @@
       <c r="B12" s="0" t="s">
         <v>46</v>
       </c>
-      <c r="C12" s="11" t="s">
+      <c r="C12" s="7" t="s">
         <v>105</v>
       </c>
       <c r="D12" s="7" t="s">
@@ -3081,7 +2969,7 @@
       </c>
       <c r="P13" s="1" t="n">
         <f aca="false">P10+P11+P12</f>
-        <v>2742</v>
+        <v>1926.78</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3091,7 +2979,7 @@
       <c r="B14" s="0" t="s">
         <v>52</v>
       </c>
-      <c r="C14" s="11" t="s">
+      <c r="C14" s="7" t="s">
         <v>106</v>
       </c>
       <c r="D14" s="7" t="s">
@@ -3143,7 +3031,7 @@
       </c>
       <c r="P14" s="1" t="n">
         <f aca="false">P4-P13</f>
-        <v>17258</v>
+        <v>18073.22</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3205,7 +3093,7 @@
       </c>
       <c r="P15" s="1" t="n">
         <f aca="false">ROUND(P14*7.75%,2)</f>
-        <v>1337.5</v>
+        <v>1400.67</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3267,7 +3155,7 @@
       </c>
       <c r="P16" s="1" t="n">
         <f aca="false">ROUND(P14*9%,2)</f>
-        <v>1553.22</v>
+        <v>1626.59</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3663,7 +3551,7 @@
       </c>
       <c r="P23" s="1" t="n">
         <f aca="false">ROUND(MAX(P4+P19-P13-P17-P21,0),0)</f>
-        <v>17308</v>
+        <v>18123</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3787,7 +3675,7 @@
       </c>
       <c r="P25" s="6" t="n">
         <f aca="false">P23-P24</f>
-        <v>17308</v>
+        <v>18123</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3849,7 +3737,7 @@
       </c>
       <c r="P26" s="1" t="n">
         <f aca="false">ROUND(MAX(P24*17%-P20,0)+P25*32%-P15,0)</f>
-        <v>4201</v>
+        <v>4399</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3859,8 +3747,8 @@
       <c r="B27" s="0" t="s">
         <v>91</v>
       </c>
-      <c r="C27" s="12" t="s">
-        <v>114</v>
+      <c r="C27" s="8" t="s">
+        <v>92</v>
       </c>
       <c r="D27" s="7" t="s">
         <v>17</v>
@@ -4021,7 +3909,7 @@
       </c>
       <c r="P29" s="10" t="n">
         <f aca="false">P2-P13-P16-P26-P27-P28</f>
-        <v>11103.78</v>
+        <v>11647.63</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4039,7 +3927,7 @@
       </c>
       <c r="E30" s="1" t="n">
         <f aca="false">ROUND(SUM(E29:P29)/12,2)</f>
-        <v>8761.17</v>
+        <v>8806.49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>